<commit_message>
Improved error handling in Access code; SVReg ROI data now includes ProcessingInformationID CWRU_ASL_SummarizeAll handles pCASL NiiReplaceValues deals better with NaN
</commit_message>
<xml_diff>
--- a/dev/t1b fitting.xlsx
+++ b/dev/t1b fitting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\todfl\Documents\Decker\MRI Processing\MRI Processing Software\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2389F165-44B6-4F35-AA9E-8AC8A19D3C77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5CCCB1-813A-412A-BA43-B128C44F675E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{14671F29-99C9-428C-B694-FFCF1B7E9969}"/>
   </bookViews>
@@ -34,12 +34,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>FiO2</t>
   </si>
   <si>
     <t>T1b</t>
+  </si>
+  <si>
+    <t>delM%</t>
+  </si>
+  <si>
+    <t>rel M</t>
+  </si>
+  <si>
+    <t>rel CBF</t>
   </si>
 </sst>
 </file>
@@ -108,36 +117,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -194,44 +173,8 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.2143006104194027E-3"/>
-                  <c:y val="7.7372206129289064E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:trendline>
             <c:spPr>
@@ -244,44 +187,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.8499484271695815E-2"/>
-                  <c:y val="-7.8427337619331142E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -348,6 +255,206 @@
         </c:dLbls>
         <c:axId val="352757024"/>
         <c:axId val="440192368"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rel M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93430000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85040000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82309999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B756-4882-B04D-5258ED8BC26D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rel CBF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0006051612903226</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0049210884353743</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0011801418439716</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9901057971014493</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B756-4882-B04D-5258ED8BC26D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="900376447"/>
+        <c:axId val="900377695"/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="352757024"/>
@@ -473,6 +580,68 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="900377695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="900376447"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="900376447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="900377695"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -481,6 +650,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1085,14 +1285,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>120649</xdr:rowOff>
     </xdr:to>
@@ -1419,100 +1619,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0043A1ED-B288-4334-90B6-420F140A0B83}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F8"/>
+      <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.2</v>
       </c>
       <c r="B2">
         <v>1660</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
       <c r="D2">
-        <f t="array" ref="D2:F5">LINEST(B2:B6,A2:A6,TRUE,TRUE)</f>
+        <f>1+C2/100</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>D2*$B$2/B2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f t="array" ref="H2:J5">LINEST(B2:B6,A2:A6,TRUE,TRUE)</f>
         <v>-350</v>
       </c>
-      <c r="E2">
+      <c r="I2">
         <v>1704</v>
       </c>
-      <c r="F2" t="e">
+      <c r="J2" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.4</v>
       </c>
       <c r="B3">
         <v>1550</v>
       </c>
+      <c r="C3">
+        <v>-6.57</v>
+      </c>
       <c r="D3">
+        <f t="shared" ref="D3:D6" si="0">1+C3/100</f>
+        <v>0.93430000000000002</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E6" si="1">D3*$B$2/B3</f>
+        <v>1.0006051612903226</v>
+      </c>
+      <c r="H3">
         <v>43.969686527576393</v>
       </c>
-      <c r="E3">
+      <c r="I3">
         <v>29.166190472303143</v>
       </c>
-      <c r="F3" t="e">
+      <c r="J3" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0.6</v>
       </c>
       <c r="B4">
         <v>1470</v>
       </c>
+      <c r="C4">
+        <v>-11.01</v>
+      </c>
       <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.88990000000000002</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>1.0049210884353743</v>
+      </c>
+      <c r="H4">
         <v>0.95479345284489481</v>
       </c>
-      <c r="E4">
+      <c r="I4">
         <v>27.808871486152281</v>
       </c>
-      <c r="F4" t="e">
+      <c r="J4" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.8</v>
       </c>
       <c r="B5">
         <v>1410</v>
       </c>
+      <c r="C5">
+        <v>-14.96</v>
+      </c>
       <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.85040000000000004</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>1.0011801418439716</v>
+      </c>
+      <c r="H5">
         <v>63.362068965517238</v>
       </c>
-      <c r="E5">
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="F5" t="e">
+      <c r="J5" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6">
         <v>1380</v>
       </c>
+      <c r="C6">
+        <v>-17.690000000000001</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.82309999999999994</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0.9901057971014493</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1520,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>

</xml_diff>